<commit_message>
Update Ozone.bg Test Cases v1.0.xlsx
</commit_message>
<xml_diff>
--- a/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
+++ b/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
     <sheet name="Landing Page" sheetId="2" r:id="rId2"/>
     <sheet name="Registration and Account" sheetId="13" r:id="rId3"/>
     <sheet name="Navigation" sheetId="14" r:id="rId4"/>
-    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId5"/>
-    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId6"/>
-    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId7"/>
-    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="Search" sheetId="15" r:id="rId5"/>
+    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId7"/>
+    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId8"/>
+    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Landing Page'!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Navigation!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Registration and Account'!$A$1:$H$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Search!$A$1:$H$47</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -89,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="315">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -1119,6 +1121,9 @@
   </si>
   <si>
     <t>User should be on "Люлки и шезлонги" products page</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
 </sst>
 </file>
@@ -1734,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:T16"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3610,7 +3615,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5077,7 +5082,7 @@
   </sheetPr>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="A21:F30"/>
     </sheetView>
@@ -6508,6 +6513,1277 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I119"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="A5:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="24" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="58.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="14.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="32" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="25"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="15"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="15"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="15"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="15"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="15"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="15"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="15"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="22"/>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="15"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="22"/>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="23"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="23"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="23"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="20"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="20"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="20"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="20"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+    </row>
+    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="20"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="20"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="20"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="20"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="20"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="20"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="20"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="20"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="20"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="20"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="20"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="20"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="20"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="20"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="20"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="20"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="20"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="20"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="20"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="20"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="20"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="20"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="20"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="20"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="20"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="20"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="20"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="20"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="20"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="20"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="20"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="20"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="20"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="20"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="20"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="20"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="20"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="20"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="20"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="20"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="20"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="20"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="20"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="20"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="20"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="20"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="20"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="20"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="20"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="20"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
+      <c r="G118" s="18"/>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="20"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+      <c r="G119" s="18"/>
+      <c r="H119" s="18"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H47"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6687,7 +7963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6781,7 +8057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -7021,7 +8297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
new test casess added
</commit_message>
<xml_diff>
--- a/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
+++ b/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -20,15 +20,17 @@
     <sheet name="Product overview" sheetId="16" r:id="rId6"/>
     <sheet name="Product Detail Page" sheetId="17" r:id="rId7"/>
     <sheet name="Cart" sheetId="18" r:id="rId8"/>
-    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId9"/>
-    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId10"/>
-    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId11"/>
-    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId12"/>
+    <sheet name="Order Process" sheetId="20" r:id="rId9"/>
+    <sheet name="FundTransfer" sheetId="3" state="hidden" r:id="rId10"/>
+    <sheet name="BalenceEnquiry" sheetId="4" state="hidden" r:id="rId11"/>
+    <sheet name="Inter Bank Fund  Transfer" sheetId="5" state="hidden" r:id="rId12"/>
+    <sheet name="Change  password" sheetId="6" state="hidden" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Cart!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Landing Page'!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Navigation!$A$1:$H$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Order Process'!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Product Detail Page'!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Product overview'!$A$1:$H$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Registration and Account'!$A$1:$H$47</definedName>
@@ -97,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="465">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -1555,12 +1557,107 @@
 2. Hover over "Категории" &gt; "Тв, монитори и видео" and click "Dell"
 3. Click "Геймърски монитор Dell S2719DGF - 27"" &gt; "Купи" &gt; "към количката"</t>
   </si>
+  <si>
+    <t>Increase quantities in cart</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Книжарница" and click "Научна фантастика, фентъзи и хорър"
+3. Click "Фолклорът на света на диска
+" &gt; "PRE-ORDER" &gt; "към количката"
+4. Click "Plus" button 10 times</t>
+  </si>
+  <si>
+    <t>Increase Фолклорът на света на диска 10 times</t>
+  </si>
+  <si>
+    <t>Increase Геймърски монитор Dell S2719DGF - 27 5 times</t>
+  </si>
+  <si>
+    <t>Increase Гейминг конфигурация White Walker 5 times</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Тв, монитори и видео" and click "Dell"
+3. Click "Геймърски монитор Dell S2719DGF" &gt; "Купи" &gt; "към количката"
+4. Click "Plus" button 5 times</t>
+  </si>
+  <si>
+    <t>Quantites increase by 10 and price increases accordingly</t>
+  </si>
+  <si>
+    <t>Quantites increase by 5 and price increases accordingly</t>
+  </si>
+  <si>
+    <t>Set quantities in cart to 0</t>
+  </si>
+  <si>
+    <t>Set quantites for Фолклорът на света на диска to 0</t>
+  </si>
+  <si>
+    <t>Item disappears from cart</t>
+  </si>
+  <si>
+    <t>Set quantites for Гейминг конфигурация White Walker to 0</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Книжарница" and click "Научна фантастика, фентъзи и хорър"
+3. Click "Фолклорът на света на диска
+" &gt; "PRE-ORDER" &gt; "към количката"
+4. Click inside the Quantites field and enter 0</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Лаптопи и компютри" and click "Ozone"
+3. Click "Гейминг конфигурация White Walker" &gt; "Купи" &gt; "към количката"
+4. Click "Plus" button 5 times</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Лаптопи и компютри" and click "Ozone"
+3. Click "Гейминг конфигурация White Walker" &gt; "Купи" &gt; "към количката"
+4. Click inside the Quantites field and enter 0</t>
+  </si>
+  <si>
+    <t>Set quantites for Геймърски монитор Dell S2719DGF to 0</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Тв, монитори и видео" and click "Dell"
+3. Click "Геймърски монитор Dell S2719DGF" &gt; "Купи" &gt; "към количката"
+4. Click inside the Quantites field and enter 0</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1677,6 +1774,21 @@
     <font>
       <u/>
       <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1798,7 +1910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1898,6 +2010,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2183,7 +2307,7 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="G38" sqref="G38:P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2535,6 +2659,190 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="7" max="19" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2628,7 +2936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2868,7 +3176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -11546,9 +11854,9 @@
   </sheetPr>
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="A8:D11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11620,7 +11928,9 @@
       <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="15" t="s">
+        <v>457</v>
+      </c>
       <c r="B3" s="17"/>
       <c r="C3" s="16" t="s">
         <v>435</v>
@@ -11640,7 +11950,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="15" t="s">
+        <v>458</v>
+      </c>
       <c r="B4" s="17"/>
       <c r="C4" s="16" t="s">
         <v>438</v>
@@ -11659,65 +11971,147 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+    <row r="5" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>441</v>
+      </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="F5" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>460</v>
+      </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>453</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="F6" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>461</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>445</v>
+      </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="F7" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="E8" s="27">
+        <v>0</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>463</v>
+      </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="C9" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>464</v>
+      </c>
       <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>456</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
@@ -12835,181 +13229,1268 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="A2:H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="19" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="24" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="58.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="14.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="I1" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="32" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2" s="39"/>
+      <c r="F2" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="25"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="15"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="15"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="15"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="15"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="15"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="15"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="15"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="22"/>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="15"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="22"/>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="23"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="23"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="23"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="20"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="20"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="20"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="20"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+    </row>
+    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="20"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="20"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="20"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="20"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="20"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="20"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="20"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="20"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="20"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="20"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="20"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="20"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="20"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="20"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="20"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="20"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="20"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="20"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="18"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="20"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="20"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="18"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="20"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="18"/>
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="20"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="20"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="20"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="20"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="20"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="20"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="20"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="20"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="20"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="18"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="20"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="20"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="18"/>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="20"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="20"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="20"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="20"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="18"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="20"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="20"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="20"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="20"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="20"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="20"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="20"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="20"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="18"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="20"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
+      <c r="G113" s="18"/>
+      <c r="H113" s="18"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="20"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="20"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="20"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="20"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="20"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
+      <c r="G118" s="18"/>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="20"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+      <c r="G119" s="18"/>
+      <c r="H119" s="18"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H47"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new test cases addded
</commit_message>
<xml_diff>
--- a/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
+++ b/E-comerse/Ozone/Ozone.bg Test Cases v1.0.xlsx
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="500">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -1652,12 +1652,126 @@
   <si>
     <t>C9</t>
   </si>
+  <si>
+    <t>OP1</t>
+  </si>
+  <si>
+    <t>Order "Това не е краят"</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Книжарница" and click "Романтични"
+3. Click "Това не е краят"&gt; "PRE-ORDER" &gt; "към количката"
+4. Click "Към Завършване"</t>
+  </si>
+  <si>
+    <t>Order a book with "Плащане в брой"</t>
+  </si>
+  <si>
+    <t>Order Lenovo Y540-15IRH</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Лаптопи и компютри" and click "Lenovo"
+3. Click "Lenovo Y540-15IRH"&gt; "Купи" &gt; "към количката"
+4. Click "Към Завършване"</t>
+  </si>
+  <si>
+    <t>Product and transport prices are visible and clear</t>
+  </si>
+  <si>
+    <t>Order Wacom Intuos Pro M, North</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.ozone.bg/
+2. Hover over "Категории" &gt; "Мобилни устройства" and click "За професионалисти"
+3. Click "Wacom Intuos Pro M, North"&gt; "Купи" &gt; "към количката"
+4. Click "Към Завършване"</t>
+  </si>
+  <si>
+    <t>Change "Начин на плащане"</t>
+  </si>
+  <si>
+    <t>Change to Epay</t>
+  </si>
+  <si>
+    <t>1. From OP3 click "Epay" from Начини на плащане</t>
+  </si>
+  <si>
+    <t>Change to ePay - EasyPay и B-Pay</t>
+  </si>
+  <si>
+    <t>1. From OP4 click "ePay - EasyPay и B-Pay" from Начини на плащане</t>
+  </si>
+  <si>
+    <t>ePay logo appears and user can pay by Epay</t>
+  </si>
+  <si>
+    <t>easy Pay logo appears and user can pay by easy Pay</t>
+  </si>
+  <si>
+    <t>Change Плащане с карта</t>
+  </si>
+  <si>
+    <t>1. From OP5 click "Плащане с карта" from Начини на плащане</t>
+  </si>
+  <si>
+    <t>Paying cards logo appears</t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t>OP3</t>
+  </si>
+  <si>
+    <t>OP4</t>
+  </si>
+  <si>
+    <t>OP5</t>
+  </si>
+  <si>
+    <t>OP6</t>
+  </si>
+  <si>
+    <t>change "Метод на доставка"</t>
+  </si>
+  <si>
+    <t>Change to "Магазин Ozone"</t>
+  </si>
+  <si>
+    <t>1. From OP6 click "Магазин Ozone" from Методи на доставка</t>
+  </si>
+  <si>
+    <t>Delivery address and price changes accordingly</t>
+  </si>
+  <si>
+    <t>Change to "Офис Speedy: 2,99 лв."</t>
+  </si>
+  <si>
+    <t>1. From OP7 click "Офис Speedy: 2,99 лв." from Методи на доставка</t>
+  </si>
+  <si>
+    <t>Change to "Офис Еконт: 2,99 лв."</t>
+  </si>
+  <si>
+    <t>1. From OP7 click "Офис Еконт: 2,99 лв." from Методи на доставка</t>
+  </si>
+  <si>
+    <t>OP7</t>
+  </si>
+  <si>
+    <t>OP8</t>
+  </si>
+  <si>
+    <t>OP9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1774,21 +1888,6 @@
     <font>
       <u/>
       <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1910,7 +2009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2010,18 +2109,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2307,7 +2394,7 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38:P39"/>
+      <selection activeCell="H44" sqref="H44:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13233,7 +13320,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="A2:H2"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13280,109 +13367,209 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="32" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>431</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>432</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>434</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>436</v>
-      </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="37" t="s">
-        <v>433</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>433</v>
-      </c>
-      <c r="H2" s="37" t="s">
+      <c r="A2" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="31"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>484</v>
+      </c>
       <c r="B3" s="17"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="16" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="E3" s="34"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="F3" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>485</v>
+      </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="16" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>473</v>
+      </c>
       <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
+      <c r="F4" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>476</v>
+      </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="F5" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>487</v>
+      </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>478</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="F6" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>488</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="16" t="s">
+        <v>481</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>482</v>
+      </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
+      <c r="F7" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>491</v>
+      </c>
       <c r="E8" s="27"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="F8" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>498</v>
+      </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="E9" s="28"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="F9" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>499</v>
+      </c>
       <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="C10" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>496</v>
+      </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>

</xml_diff>